<commit_message>
Payday Reporting * Employer events table - Updated to include new Event Type * ES Build Pack - Updated to include new Event Type * ES Events Sample Payloads - Updated * EI Build Pack v1 - Updated to include new Response Code * EI Build Pack v2 - Updated to include new Response Code
</commit_message>
<xml_diff>
--- a/Service - Payday Filing/Employee Details/sample messages/ES-Events-Sample-Payloads.xlsx
+++ b/Service - Payday Filing/Employee Details/sample messages/ES-Events-Sample-Payloads.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://irnz-my.sharepoint.com/personal/david_shackleton_ird_govt_nz/Documents/Desktop/S4-1-2 Mocks/Employment Service/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://irnz-my.sharepoint.com/personal/james_bowen_ird_govt_nz/Documents/GIT REPO/Gateway Services/gateway_services-returns-and-information/Service - Payday Filing/Employee Details/sample messages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{841A3488-646C-42EC-8605-57A2A0D80434}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{87B1ADA4-CEA0-41BD-B060-B12FC8F7B009}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{841A3488-646C-42EC-8605-57A2A0D80434}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5DC7B923-533F-4ADC-9A2F-2F3086605A9F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{767AD0F5-F2F2-46FD-8622-1B46A93B8205}"/>
+    <workbookView xWindow="-4995" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{767AD0F5-F2F2-46FD-8622-1B46A93B8205}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1467,14 +1467,14 @@
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="95.42578125" customWidth="1"/>
-    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.42578125" customWidth="1"/>
     <col min="5" max="5" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>